<commit_message>
UnitTest TestCaseStepFilePathUtils: Extra test for TestCaseStepFilePathUtils and test analysis sheet.
</commit_message>
<xml_diff>
--- a/UnitTest/StfUtils/Doc/StfUtilsTemplateConfigUtilsUnitTestAnalysis.xlsx
+++ b/UnitTest/StfUtils/Doc/StfUtilsTemplateConfigUtilsUnitTestAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Stf\UnitTest\StfUtils\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739EDC93-81AF-4E0A-9351-FDECA720D524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DBCE0-C2D3-4F0C-A464-E3126DF393A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{E0C8DBB2-6D73-4406-A380-317E4F3CFA86}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -112,6 +112,36 @@
   </si>
   <si>
     <t>Four Steps,  Two Template, Three Config</t>
+  </si>
+  <si>
+    <t>Four Steps File Text,   Three Template, Three Config</t>
+  </si>
+  <si>
+    <t>Template2_Uscore3.txt</t>
+  </si>
+  <si>
+    <t>Template3 spaces 2.txt</t>
+  </si>
+  <si>
+    <t>Config2WithNoGap1.txt</t>
+  </si>
+  <si>
+    <t>Config4.extra.dots.12.txt</t>
+  </si>
+  <si>
+    <t>XML Template, txt config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra step in unit test case </t>
+  </si>
+  <si>
+    <t>Text in filename for 1 step</t>
+  </si>
+  <si>
+    <t>Text in filename but incorrect e.g. Template.txt ..step 2 Template 2.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More tests </t>
   </si>
 </sst>
 </file>
@@ -169,16 +199,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,21 +536,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39419D11-A7FC-438E-B514-00B47883D239}">
-  <dimension ref="A2:J34"/>
+  <dimension ref="A2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
@@ -517,39 +559,39 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="F3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -575,7 +617,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C6">
@@ -601,18 +643,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
@@ -655,18 +697,18 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -712,18 +754,18 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C14">
@@ -769,18 +811,18 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C17">
@@ -846,18 +888,18 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C21">
@@ -943,18 +985,18 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C26">
@@ -1037,18 +1079,18 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C31">
@@ -1090,7 +1132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>3</v>
       </c>
@@ -1110,7 +1152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>4</v>
       </c>
@@ -1128,6 +1170,139 @@
       </c>
       <c r="J34" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>4433</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>27</v>
+      </c>
+      <c r="J37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
StfUtils Unit Tests TestCaseStepFilePathUtils: Added Tc4331 and Tc43311
</commit_message>
<xml_diff>
--- a/UnitTest/StfUtils/Doc/StfUtilsTemplateConfigUtilsUnitTestAnalysis.xlsx
+++ b/UnitTest/StfUtils/Doc/StfUtilsTemplateConfigUtilsUnitTestAnalysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Stf\UnitTest\StfUtils\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DBCE0-C2D3-4F0C-A464-E3126DF393A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F28616A-5B08-4AC8-9941-14683D27898A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{E0C8DBB2-6D73-4406-A380-317E4F3CFA86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0C8DBB2-6D73-4406-A380-317E4F3CFA86}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseStepFilePathUtils" sheetId="2" r:id="rId1"/>
+    <sheet name="More tests " sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="39">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -142,6 +143,15 @@
   </si>
   <si>
     <t xml:space="preserve">More tests </t>
+  </si>
+  <si>
+    <t>Template.xml</t>
+  </si>
+  <si>
+    <t>Template3.json</t>
+  </si>
+  <si>
+    <t>XML Json, Tthree Template, Two Config</t>
   </si>
 </sst>
 </file>
@@ -208,9 +218,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -221,6 +228,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,16 +546,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39419D11-A7FC-438E-B514-00B47883D239}">
-  <dimension ref="A2:J46"/>
+  <dimension ref="A2:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -559,28 +569,28 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="9"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
         <v>15</v>
@@ -591,7 +601,7 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -617,7 +627,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C6">
@@ -643,7 +653,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -654,7 +664,7 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C8">
@@ -697,7 +707,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -708,7 +718,7 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -754,7 +764,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -765,7 +775,7 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C14">
@@ -811,7 +821,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -822,7 +832,7 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C17">
@@ -888,7 +898,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -899,7 +909,7 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C21">
@@ -985,7 +995,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -996,7 +1006,7 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C26">
@@ -1079,7 +1089,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1090,7 +1100,7 @@
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C31">
@@ -1173,7 +1183,7 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1184,7 +1194,7 @@
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C36">
@@ -1270,7 +1280,7 @@
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1280,29 +1290,67 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41">
+        <v>4331</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>35</v>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
-        <v>34</v>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+      <c r="J43" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1314,4 +1362,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FFCF60-EEA4-42C8-80B8-97DF48BEEEA8}">
+  <dimension ref="B3:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "StfUtils Unit Tests TestCaseStepFilePathUtils: Added Tc4331 and Tc43311"
This reverts commit 0ad8c016fec7772da58edbf4b379d05bec824a32.
</commit_message>
<xml_diff>
--- a/UnitTest/StfUtils/Doc/StfUtilsTemplateConfigUtilsUnitTestAnalysis.xlsx
+++ b/UnitTest/StfUtils/Doc/StfUtilsTemplateConfigUtilsUnitTestAnalysis.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Stf\UnitTest\StfUtils\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F28616A-5B08-4AC8-9941-14683D27898A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DBCE0-C2D3-4F0C-A464-E3126DF393A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0C8DBB2-6D73-4406-A380-317E4F3CFA86}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{E0C8DBB2-6D73-4406-A380-317E4F3CFA86}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseStepFilePathUtils" sheetId="2" r:id="rId1"/>
-    <sheet name="More tests " sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -143,15 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">More tests </t>
-  </si>
-  <si>
-    <t>Template.xml</t>
-  </si>
-  <si>
-    <t>Template3.json</t>
-  </si>
-  <si>
-    <t>XML Json, Tthree Template, Two Config</t>
   </si>
 </sst>
 </file>
@@ -218,6 +208,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -228,9 +221,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,16 +536,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39419D11-A7FC-438E-B514-00B47883D239}">
-  <dimension ref="A2:J43"/>
+  <dimension ref="A2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -569,28 +559,28 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="5"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
         <v>15</v>
@@ -601,7 +591,7 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -627,7 +617,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C6">
@@ -653,7 +643,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -664,7 +654,7 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C8">
@@ -707,7 +697,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -718,7 +708,7 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C11">
@@ -764,7 +754,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -775,7 +765,7 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C14">
@@ -821,7 +811,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -832,7 +822,7 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C17">
@@ -898,7 +888,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -909,7 +899,7 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C21">
@@ -995,7 +985,7 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1006,7 +996,7 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C26">
@@ -1089,7 +1079,7 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1100,7 +1090,7 @@
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C31">
@@ -1183,7 +1173,7 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1194,7 +1184,7 @@
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C36">
@@ -1280,7 +1270,7 @@
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1290,67 +1280,29 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41">
-        <v>4331</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" t="s">
-        <v>3</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>36</v>
-      </c>
-      <c r="J41" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" t="s">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>2</v>
-      </c>
-      <c r="I42" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" t="s">
-        <v>3</v>
+      <c r="B42" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D43">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>37</v>
-      </c>
-      <c r="H43">
-        <v>3</v>
-      </c>
-      <c r="I43" t="s">
-        <v>37</v>
-      </c>
-      <c r="J43" t="s">
-        <v>3</v>
+      <c r="B43" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1362,47 +1314,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FFCF60-EEA4-42C8-80B8-97DF48BEEEA8}">
-  <dimension ref="B3:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>